<commit_message>
first pass IO list
</commit_message>
<xml_diff>
--- a/Engine IO.xlsx
+++ b/Engine IO.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jaidan/Dropbox/Geekery/bedford330/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4685A1D-CADB-A84E-8A3A-491EF01BE3EB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E26BF8A-9D41-A148-A0D1-401C76CFB6A8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="460" windowWidth="26580" windowHeight="25140" xr2:uid="{B7C4ACD1-65CD-8348-B488-7E43C24D871F}"/>
+    <workbookView xWindow="2080" yWindow="2940" windowWidth="26580" windowHeight="25140" xr2:uid="{B7C4ACD1-65CD-8348-B488-7E43C24D871F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames>
+    <definedName name="type">Sheet1!$D$5:$D$75</definedName>
+  </definedNames>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,16 +28,118 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
   <si>
     <t>Bedford 330 Diesel I/O List</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>AI</t>
+  </si>
+  <si>
+    <t>roadSpeed</t>
+  </si>
+  <si>
+    <t>engineSpeed</t>
+  </si>
+  <si>
+    <t>fuelLevel2</t>
+  </si>
+  <si>
+    <t>fuelLevel1</t>
+  </si>
+  <si>
+    <t>waterTemp</t>
+  </si>
+  <si>
+    <t>oilTemp</t>
+  </si>
+  <si>
+    <t>oilPressure</t>
+  </si>
+  <si>
+    <t>brakePressure</t>
+  </si>
+  <si>
+    <t>engineBattVolts</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>VDO resistive sender</t>
+  </si>
+  <si>
+    <t>voltage divider</t>
+  </si>
+  <si>
+    <t>AO</t>
+  </si>
+  <si>
+    <t>waterGauge</t>
+  </si>
+  <si>
+    <t>fuelGauge</t>
+  </si>
+  <si>
+    <t>oilPressureLight</t>
+  </si>
+  <si>
+    <t>otherLight</t>
+  </si>
+  <si>
+    <t>DO</t>
+  </si>
+  <si>
+    <t>oilPressureLow</t>
+  </si>
+  <si>
+    <t>DI</t>
+  </si>
+  <si>
+    <t>brakePressureLow</t>
+  </si>
+  <si>
+    <t>IO Type</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>rpiLink</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>Smart Display</t>
+  </si>
+  <si>
+    <t>future</t>
+  </si>
+  <si>
+    <t>bluetoothLink</t>
+  </si>
+  <si>
+    <t>16:2 display</t>
+  </si>
+  <si>
+    <t>Used as backup for when Smart Display isn't working.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -42,16 +147,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -59,12 +177,118 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color theme="9"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="9"/>
+      </right>
+      <top style="medium">
+        <color theme="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="9"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="9"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="9"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="9"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,18 +603,395 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A602C23B-CEC5-164C-8B31-8A986162D4D5}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="47.6640625" customWidth="1"/>
+    <col min="6" max="6" width="1.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
+    </row>
+    <row r="3" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="11">
+        <f>COUNTIF(type, G5)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="12">
+        <f>COUNTIF(type, G6)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="12">
+        <f>COUNTIF(type, G7)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="12">
+        <f>COUNTIF(type, G8)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="13">
+        <f>COUNTIF(type, G9)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="8"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="8"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="8"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="8"/>
+      <c r="D19" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="8"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="8"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="8"/>
+      <c r="D21" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="8"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="D22" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="8"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B23" s="2"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="8"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B24" s="2"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="8"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B25" s="2"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="8"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B26" s="2"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="8"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B27" s="2"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="8"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B28" s="2"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="8"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B29" s="2"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="8"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B30" s="2"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="8"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B31" s="2"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="8"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B32" s="2"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="8"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B33" s="2"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="8"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B34" s="2"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="8"/>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B35" s="2"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="8"/>
+    </row>
+    <row r="36" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="4"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update to open xml
</commit_message>
<xml_diff>
--- a/Engine IO.xlsx
+++ b/Engine IO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jaidan/Dropbox/Geekery/bedford330/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A2F1785-80B7-0F4A-86BD-00D003D76563}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0E23B52C-D033-8642-AFD6-79E294737E19}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2080" yWindow="2940" windowWidth="26580" windowHeight="25140" xr2:uid="{B7C4ACD1-65CD-8348-B488-7E43C24D871F}"/>
   </bookViews>
@@ -20,6 +20,9 @@
   </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="58" uniqueCount="35">
   <si>
     <t>Bedford 330 Diesel I/O List</t>
   </si>
@@ -138,7 +141,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -179,17 +182,17 @@
   </fills>
   <borders count="9">
     <border>
-      <left/>
-      <right/>
+      <start/>
+      <end/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color theme="9"/>
-      </left>
-      <right/>
+      <start style="medium">
+        <color theme="9"/>
+      </start>
+      <end/>
       <top style="medium">
         <color theme="9"/>
       </top>
@@ -197,10 +200,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color theme="9"/>
-      </right>
+      <start/>
+      <end style="medium">
+        <color theme="9"/>
+      </end>
       <top style="medium">
         <color theme="9"/>
       </top>
@@ -208,28 +211,28 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color theme="9"/>
-      </left>
-      <right/>
+      <start style="medium">
+        <color theme="9"/>
+      </start>
+      <end/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color theme="9"/>
-      </right>
+      <start/>
+      <end style="medium">
+        <color theme="9"/>
+      </end>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color theme="9"/>
-      </left>
-      <right/>
+      <start style="medium">
+        <color theme="9"/>
+      </start>
+      <end/>
       <top/>
       <bottom style="medium">
         <color theme="9"/>
@@ -237,10 +240,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color theme="9"/>
-      </right>
+      <start/>
+      <end style="medium">
+        <color theme="9"/>
+      </end>
       <top/>
       <bottom style="medium">
         <color theme="9"/>
@@ -248,8 +251,8 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <start/>
+      <end/>
       <top style="medium">
         <color theme="9"/>
       </top>
@@ -257,8 +260,8 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <start/>
+      <end/>
       <top/>
       <bottom style="medium">
         <color theme="9"/>
@@ -316,7 +319,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -469,25 +472,25 @@
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <a:gs pos="0%">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:lumMod val="110%"/>
+                <a:satMod val="105%"/>
+                <a:tint val="67%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="50%">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:lumMod val="105%"/>
+                <a:satMod val="103%"/>
+                <a:tint val="73%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100000">
+            <a:gs pos="100%">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:lumMod val="105%"/>
+                <a:satMod val="109%"/>
+                <a:tint val="81%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -495,25 +498,25 @@
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <a:gs pos="0%">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:satMod val="103%"/>
+                <a:lumMod val="102%"/>
+                <a:tint val="94%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="50%">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:satMod val="110%"/>
+                <a:lumMod val="100%"/>
+                <a:shade val="100%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100000">
+            <a:gs pos="100%">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:lumMod val="99%"/>
+                <a:satMod val="120%"/>
+                <a:shade val="78%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -526,21 +529,21 @@
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter lim="800%"/>
         </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter lim="800%"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter lim="800%"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -554,7 +557,7 @@
           <a:effectLst>
             <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="63%"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -566,32 +569,32 @@
         </a:solidFill>
         <a:solidFill>
           <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
+            <a:tint val="95%"/>
+            <a:satMod val="170%"/>
           </a:schemeClr>
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <a:gs pos="0%">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="93%"/>
+                <a:satMod val="150%"/>
+                <a:shade val="98%"/>
+                <a:lumMod val="102%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="50%">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="98%"/>
+                <a:satMod val="130%"/>
+                <a:shade val="90%"/>
+                <a:lumMod val="103%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100000">
+            <a:gs pos="100%">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="63%"/>
+                <a:satMod val="120%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -611,7 +614,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A602C23B-CEC5-164C-8B31-8A986162D4D5}">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A602C23B-CEC5-164C-8B31-8A986162D4D5}">
   <dimension ref="B2:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">

</xml_diff>

<commit_message>
update attributes to make excel file work with versioning
</commit_message>
<xml_diff>
--- a/Engine IO.xlsx
+++ b/Engine IO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jaidan/Dropbox/Geekery/bedford330/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0E23B52C-D033-8642-AFD6-79E294737E19}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{ED263B70-CEC9-7443-9A7C-224BE2455DBF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2080" yWindow="2940" windowWidth="26580" windowHeight="25140" xr2:uid="{B7C4ACD1-65CD-8348-B488-7E43C24D871F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="58" uniqueCount="35">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="61" uniqueCount="37">
   <si>
     <t>Bedford 330 Diesel I/O List</t>
   </si>
@@ -136,6 +136,12 @@
   </si>
   <si>
     <t>Used as backup for when Smart Display isn't working.</t>
+  </si>
+  <si>
+    <t>housePowerLink</t>
+  </si>
+  <si>
+    <t>comms link with the house power battery monitor</t>
   </si>
 </sst>
 </file>
@@ -618,7 +624,7 @@
   <dimension ref="B2:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -752,7 +758,7 @@
       </c>
       <c r="H9" s="13">
         <f>COUNTIF(type, G9)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
@@ -908,10 +914,16 @@
       <c r="F22" s="8"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B23" s="2"/>
+      <c r="B23" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="3"/>
+      <c r="D23" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="F23" s="8"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.2">

</xml_diff>